<commit_message>
Selling functionlity finished, now stored in database.
</commit_message>
<xml_diff>
--- a/Documents/Laker Books Gantt Chart.xlsx
+++ b/Documents/Laker Books Gantt Chart.xlsx
@@ -197,7 +197,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF8DB4E2"/>
+        <fgColor theme="3" tint="-0.249977111117893"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -734,8 +734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CZ41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="I5" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="Y17" sqref="Y17:AC17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1216,40 +1216,40 @@
       <c r="A13" t="s">
         <v>16</v>
       </c>
-      <c r="R13" s="4"/>
-      <c r="S13" s="4"/>
-      <c r="T13" s="4"/>
-      <c r="U13" s="4"/>
-      <c r="V13" s="4"/>
-      <c r="W13" s="4"/>
-      <c r="X13" s="4"/>
+      <c r="R13" s="3"/>
+      <c r="S13" s="3"/>
+      <c r="T13" s="3"/>
+      <c r="U13" s="3"/>
+      <c r="V13" s="3"/>
+      <c r="W13" s="3"/>
+      <c r="X13" s="3"/>
     </row>
     <row r="14" spans="1:104">
       <c r="B14" t="s">
         <v>15</v>
       </c>
-      <c r="R14" s="4"/>
-      <c r="S14" s="4"/>
-      <c r="T14" s="4"/>
+      <c r="R14" s="3"/>
+      <c r="S14" s="3"/>
+      <c r="T14" s="3"/>
     </row>
     <row r="15" spans="1:104">
       <c r="B15" t="s">
         <v>14</v>
       </c>
       <c r="U15" s="5"/>
-      <c r="V15" s="4"/>
-      <c r="W15" s="4"/>
-      <c r="X15" s="4"/>
+      <c r="V15" s="3"/>
+      <c r="W15" s="3"/>
+      <c r="X15" s="3"/>
     </row>
     <row r="17" spans="1:79">
       <c r="A17" t="s">
         <v>17</v>
       </c>
-      <c r="Y17" s="4"/>
-      <c r="Z17" s="4"/>
-      <c r="AA17" s="4"/>
-      <c r="AB17" s="4"/>
-      <c r="AC17" s="4"/>
+      <c r="Y17" s="3"/>
+      <c r="Z17" s="3"/>
+      <c r="AA17" s="3"/>
+      <c r="AB17" s="3"/>
+      <c r="AC17" s="3"/>
       <c r="AD17" s="4"/>
       <c r="AE17" s="4"/>
       <c r="AF17" s="4"/>
@@ -1271,11 +1271,11 @@
       <c r="B18" t="s">
         <v>21</v>
       </c>
-      <c r="Y18" s="4"/>
-      <c r="Z18" s="4"/>
-      <c r="AA18" s="4"/>
-      <c r="AB18" s="4"/>
-      <c r="AC18" s="4"/>
+      <c r="Y18" s="3"/>
+      <c r="Z18" s="3"/>
+      <c r="AA18" s="3"/>
+      <c r="AB18" s="3"/>
+      <c r="AC18" s="3"/>
       <c r="AD18" s="4"/>
       <c r="AE18" s="4"/>
       <c r="AF18" s="4"/>

</xml_diff>

<commit_message>
GUI was improved and made mobile friendly by using bootstrap
</commit_message>
<xml_diff>
--- a/Documents/Laker Books Gantt Chart.xlsx
+++ b/Documents/Laker Books Gantt Chart.xlsx
@@ -734,8 +734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CZ41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I5" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="Y17" sqref="Y17:AC17"/>
+    <sheetView tabSelected="1" topLeftCell="AK5" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="AT22" sqref="AT22:AZ23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1250,22 +1250,22 @@
       <c r="AA17" s="3"/>
       <c r="AB17" s="3"/>
       <c r="AC17" s="3"/>
-      <c r="AD17" s="4"/>
-      <c r="AE17" s="4"/>
-      <c r="AF17" s="4"/>
-      <c r="AG17" s="4"/>
-      <c r="AH17" s="4"/>
-      <c r="AI17" s="4"/>
-      <c r="AJ17" s="4"/>
-      <c r="AK17" s="4"/>
-      <c r="AL17" s="4"/>
-      <c r="AM17" s="4"/>
-      <c r="AN17" s="4"/>
-      <c r="AO17" s="4"/>
-      <c r="AP17" s="4"/>
-      <c r="AQ17" s="4"/>
-      <c r="AR17" s="4"/>
-      <c r="AS17" s="4"/>
+      <c r="AD17" s="3"/>
+      <c r="AE17" s="3"/>
+      <c r="AF17" s="3"/>
+      <c r="AG17" s="3"/>
+      <c r="AH17" s="3"/>
+      <c r="AI17" s="3"/>
+      <c r="AJ17" s="3"/>
+      <c r="AK17" s="3"/>
+      <c r="AL17" s="3"/>
+      <c r="AM17" s="3"/>
+      <c r="AN17" s="3"/>
+      <c r="AO17" s="3"/>
+      <c r="AP17" s="3"/>
+      <c r="AQ17" s="3"/>
+      <c r="AR17" s="3"/>
+      <c r="AS17" s="3"/>
     </row>
     <row r="18" spans="1:79">
       <c r="B18" t="s">
@@ -1276,44 +1276,44 @@
       <c r="AA18" s="3"/>
       <c r="AB18" s="3"/>
       <c r="AC18" s="3"/>
-      <c r="AD18" s="4"/>
-      <c r="AE18" s="4"/>
-      <c r="AF18" s="4"/>
-      <c r="AG18" s="4"/>
-      <c r="AH18" s="4"/>
+      <c r="AD18" s="3"/>
+      <c r="AE18" s="3"/>
+      <c r="AF18" s="3"/>
+      <c r="AG18" s="3"/>
+      <c r="AH18" s="3"/>
     </row>
     <row r="19" spans="1:79">
       <c r="B19" t="s">
         <v>22</v>
       </c>
-      <c r="AI19" s="4"/>
-      <c r="AJ19" s="4"/>
-      <c r="AK19" s="4"/>
-      <c r="AL19" s="4"/>
-      <c r="AM19" s="4"/>
-      <c r="AN19" s="4"/>
-      <c r="AO19" s="4"/>
+      <c r="AI19" s="3"/>
+      <c r="AJ19" s="3"/>
+      <c r="AK19" s="3"/>
+      <c r="AL19" s="3"/>
+      <c r="AM19" s="3"/>
+      <c r="AN19" s="3"/>
+      <c r="AO19" s="3"/>
     </row>
     <row r="20" spans="1:79">
       <c r="B20" t="s">
         <v>25</v>
       </c>
-      <c r="AP20" s="4"/>
-      <c r="AQ20" s="4"/>
-      <c r="AR20" s="4"/>
-      <c r="AS20" s="4"/>
+      <c r="AP20" s="3"/>
+      <c r="AQ20" s="3"/>
+      <c r="AR20" s="3"/>
+      <c r="AS20" s="3"/>
     </row>
     <row r="22" spans="1:79">
       <c r="A22" t="s">
         <v>20</v>
       </c>
-      <c r="AT22" s="4"/>
-      <c r="AU22" s="4"/>
-      <c r="AV22" s="4"/>
-      <c r="AW22" s="4"/>
-      <c r="AX22" s="4"/>
-      <c r="AY22" s="4"/>
-      <c r="AZ22" s="4"/>
+      <c r="AT22" s="3"/>
+      <c r="AU22" s="3"/>
+      <c r="AV22" s="3"/>
+      <c r="AW22" s="3"/>
+      <c r="AX22" s="3"/>
+      <c r="AY22" s="3"/>
+      <c r="AZ22" s="3"/>
       <c r="BA22" s="4"/>
       <c r="BB22" s="4"/>
       <c r="BC22" s="4"/>
@@ -1328,13 +1328,13 @@
       <c r="B23" t="s">
         <v>19</v>
       </c>
-      <c r="AT23" s="4"/>
-      <c r="AU23" s="4"/>
-      <c r="AV23" s="4"/>
-      <c r="AW23" s="4"/>
-      <c r="AX23" s="4"/>
-      <c r="AY23" s="4"/>
-      <c r="AZ23" s="4"/>
+      <c r="AT23" s="3"/>
+      <c r="AU23" s="3"/>
+      <c r="AV23" s="3"/>
+      <c r="AW23" s="3"/>
+      <c r="AX23" s="3"/>
+      <c r="AY23" s="3"/>
+      <c r="AZ23" s="3"/>
     </row>
     <row r="24" spans="1:79">
       <c r="B24" t="s">

</xml_diff>

<commit_message>
Made a change to gantt chart to reflect finishing touches done to backend functionality this week
</commit_message>
<xml_diff>
--- a/Documents/Laker Books Gantt Chart.xlsx
+++ b/Documents/Laker Books Gantt Chart.xlsx
@@ -96,9 +96,6 @@
     <t>Make GUI mobile-friendly &amp; test on devices</t>
   </si>
   <si>
-    <t>Allow pictures to be taken and uploaded</t>
-  </si>
-  <si>
     <t>Create final application logo</t>
   </si>
   <si>
@@ -130,6 +127,9 @@
   </si>
   <si>
     <t>Create GUI Skeleton</t>
+  </si>
+  <si>
+    <t>Finish backend functionality</t>
   </si>
 </sst>
 </file>
@@ -734,8 +734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CZ41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AK5" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="AT22" sqref="AT22:AZ23"/>
+    <sheetView tabSelected="1" topLeftCell="AJ7" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1203,7 +1203,7 @@
     </row>
     <row r="11" spans="1:104">
       <c r="B11" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
@@ -1281,6 +1281,10 @@
       <c r="AF18" s="3"/>
       <c r="AG18" s="3"/>
       <c r="AH18" s="3"/>
+      <c r="AP18" s="3"/>
+      <c r="AQ18" s="3"/>
+      <c r="AR18" s="3"/>
+      <c r="AS18" s="3"/>
     </row>
     <row r="19" spans="1:79">
       <c r="B19" t="s">
@@ -1294,18 +1298,30 @@
       <c r="AN19" s="3"/>
       <c r="AO19" s="3"/>
     </row>
-    <row r="20" spans="1:79">
-      <c r="B20" t="s">
-        <v>25</v>
-      </c>
-      <c r="AP20" s="3"/>
-      <c r="AQ20" s="3"/>
-      <c r="AR20" s="3"/>
-      <c r="AS20" s="3"/>
+    <row r="21" spans="1:79">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+      <c r="AT21" s="3"/>
+      <c r="AU21" s="3"/>
+      <c r="AV21" s="3"/>
+      <c r="AW21" s="3"/>
+      <c r="AX21" s="3"/>
+      <c r="AY21" s="3"/>
+      <c r="AZ21" s="3"/>
+      <c r="BA21" s="4"/>
+      <c r="BB21" s="4"/>
+      <c r="BC21" s="4"/>
+      <c r="BD21" s="4"/>
+      <c r="BE21" s="4"/>
+      <c r="BF21" s="4"/>
+      <c r="BG21" s="4"/>
+      <c r="BH21" s="4"/>
+      <c r="BI21" s="4"/>
     </row>
     <row r="22" spans="1:79">
-      <c r="A22" t="s">
-        <v>20</v>
+      <c r="B22" t="s">
+        <v>19</v>
       </c>
       <c r="AT22" s="3"/>
       <c r="AU22" s="3"/>
@@ -1314,19 +1330,10 @@
       <c r="AX22" s="3"/>
       <c r="AY22" s="3"/>
       <c r="AZ22" s="3"/>
-      <c r="BA22" s="4"/>
-      <c r="BB22" s="4"/>
-      <c r="BC22" s="4"/>
-      <c r="BD22" s="4"/>
-      <c r="BE22" s="4"/>
-      <c r="BF22" s="4"/>
-      <c r="BG22" s="4"/>
-      <c r="BH22" s="4"/>
-      <c r="BI22" s="4"/>
     </row>
     <row r="23" spans="1:79">
       <c r="B23" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="AT23" s="3"/>
       <c r="AU23" s="3"/>
@@ -1389,14 +1396,14 @@
     </row>
     <row r="29" spans="1:79">
       <c r="B29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="BN29" s="4"/>
       <c r="BO29" s="4"/>
     </row>
     <row r="30" spans="1:79">
       <c r="B30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="BP30" s="4"/>
       <c r="BQ30" s="4"/>
@@ -1406,12 +1413,12 @@
     </row>
     <row r="32" spans="1:79">
       <c r="A32" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="33" spans="1:103">
       <c r="B33" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="BU33" s="4"/>
       <c r="BV33" s="4"/>
@@ -1423,7 +1430,7 @@
     </row>
     <row r="35" spans="1:103">
       <c r="A35" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="CB35" s="4"/>
       <c r="CC35" s="4"/>
@@ -1435,7 +1442,7 @@
     </row>
     <row r="36" spans="1:103">
       <c r="B36" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="CB36" s="4"/>
       <c r="CC36" s="4"/>
@@ -1443,7 +1450,7 @@
     </row>
     <row r="37" spans="1:103">
       <c r="B37" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="CE37" s="4"/>
       <c r="CF37" s="4"/>
@@ -1452,12 +1459,12 @@
     </row>
     <row r="39" spans="1:103">
       <c r="A39" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="40" spans="1:103">
       <c r="B40" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="CN40" s="4"/>
       <c r="CO40" s="4"/>
@@ -1467,7 +1474,7 @@
     </row>
     <row r="41" spans="1:103">
       <c r="B41" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="CS41" s="4"/>
       <c r="CT41" s="4"/>

</xml_diff>

<commit_message>
Added authentication through oswego emails, and number formatting
</commit_message>
<xml_diff>
--- a/Documents/Laker Books Gantt Chart.xlsx
+++ b/Documents/Laker Books Gantt Chart.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14400" tabRatio="500"/>
@@ -176,7 +176,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -201,6 +201,12 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF8DB4E2"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -211,7 +217,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="91">
+  <cellStyleXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -303,16 +309,33 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="91">
+  <cellStyles count="107">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -358,6 +381,14 @@
     <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -403,6 +434,14 @@
     <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -734,8 +773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CZ41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AJ7" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="BI20" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="BU31" sqref="BU31:BW31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1309,15 +1348,15 @@
       <c r="AX21" s="3"/>
       <c r="AY21" s="3"/>
       <c r="AZ21" s="3"/>
-      <c r="BA21" s="4"/>
-      <c r="BB21" s="4"/>
-      <c r="BC21" s="4"/>
-      <c r="BD21" s="4"/>
-      <c r="BE21" s="4"/>
-      <c r="BF21" s="4"/>
-      <c r="BG21" s="4"/>
-      <c r="BH21" s="4"/>
-      <c r="BI21" s="4"/>
+      <c r="BA21" s="3"/>
+      <c r="BB21" s="3"/>
+      <c r="BC21" s="3"/>
+      <c r="BD21" s="3"/>
+      <c r="BE21" s="3"/>
+      <c r="BF21" s="3"/>
+      <c r="BG21" s="3"/>
+      <c r="BH21" s="3"/>
+      <c r="BI21" s="3"/>
     </row>
     <row r="22" spans="1:79">
       <c r="B22" t="s">
@@ -1347,86 +1386,93 @@
       <c r="B24" t="s">
         <v>24</v>
       </c>
-      <c r="BA24" s="4"/>
-      <c r="BB24" s="4"/>
-      <c r="BC24" s="4"/>
-      <c r="BD24" s="4"/>
-      <c r="BE24" s="4"/>
-    </row>
-    <row r="25" spans="1:79">
-      <c r="B25" t="s">
-        <v>18</v>
-      </c>
-      <c r="BF25" s="4"/>
-      <c r="BG25" s="4"/>
-      <c r="BH25" s="4"/>
-      <c r="BI25" s="4"/>
+      <c r="BA24" s="3"/>
+      <c r="BB24" s="3"/>
+      <c r="BC24" s="3"/>
+      <c r="BD24" s="3"/>
+      <c r="BE24" s="3"/>
+      <c r="BF24" s="3"/>
+      <c r="BG24" s="3"/>
+      <c r="BH24" s="3"/>
+      <c r="BI24" s="3"/>
+    </row>
+    <row r="26" spans="1:79">
+      <c r="A26" t="s">
+        <v>23</v>
+      </c>
+      <c r="BJ26" s="3"/>
+      <c r="BK26" s="3"/>
+      <c r="BL26" s="3"/>
+      <c r="BM26" s="3"/>
+      <c r="BN26" s="3"/>
+      <c r="BO26" s="3"/>
+      <c r="BP26" s="3"/>
+      <c r="BQ26" s="3"/>
+      <c r="BR26" s="3"/>
+      <c r="BS26" s="3"/>
+      <c r="BT26" s="3"/>
     </row>
     <row r="27" spans="1:79">
-      <c r="A27" t="s">
-        <v>23</v>
-      </c>
-      <c r="BJ27" s="4"/>
-      <c r="BK27" s="4"/>
-      <c r="BL27" s="4"/>
-      <c r="BM27" s="4"/>
-      <c r="BN27" s="4"/>
-      <c r="BO27" s="4"/>
-      <c r="BP27" s="4"/>
-      <c r="BQ27" s="4"/>
-      <c r="BR27" s="4"/>
-      <c r="BS27" s="4"/>
-      <c r="BT27" s="4"/>
-      <c r="BU27" s="4"/>
-      <c r="BV27" s="4"/>
-      <c r="BW27" s="4"/>
-      <c r="BX27" s="4"/>
-      <c r="BY27" s="4"/>
-      <c r="BZ27" s="4"/>
-      <c r="CA27" s="4"/>
+      <c r="B27" t="s">
+        <v>13</v>
+      </c>
+      <c r="BJ27" s="3"/>
+      <c r="BK27" s="3"/>
+      <c r="BL27" s="3"/>
+      <c r="BM27" s="3"/>
+      <c r="BN27" s="3"/>
+      <c r="BO27" s="3"/>
+      <c r="BP27" s="3"/>
+      <c r="BQ27" s="3"/>
+      <c r="BR27" s="3"/>
     </row>
     <row r="28" spans="1:79">
       <c r="B28" t="s">
-        <v>13</v>
-      </c>
-      <c r="BJ28" s="4"/>
-      <c r="BK28" s="4"/>
-      <c r="BL28" s="4"/>
-      <c r="BM28" s="4"/>
-    </row>
-    <row r="29" spans="1:79">
-      <c r="B29" t="s">
         <v>25</v>
       </c>
-      <c r="BN29" s="4"/>
-      <c r="BO29" s="4"/>
+      <c r="BS28" s="3"/>
+      <c r="BT28" s="3"/>
     </row>
     <row r="30" spans="1:79">
-      <c r="B30" t="s">
-        <v>26</v>
-      </c>
-      <c r="BP30" s="4"/>
-      <c r="BQ30" s="4"/>
-      <c r="BR30" s="4"/>
-      <c r="BS30" s="4"/>
-      <c r="BT30" s="4"/>
+      <c r="A30" t="s">
+        <v>27</v>
+      </c>
+      <c r="BU30" s="4"/>
+      <c r="BV30" s="4"/>
+      <c r="BW30" s="4"/>
+      <c r="BX30" s="4"/>
+      <c r="BY30" s="4"/>
+      <c r="BZ30" s="4"/>
+      <c r="CA30" s="4"/>
+    </row>
+    <row r="31" spans="1:79">
+      <c r="B31" t="s">
+        <v>28</v>
+      </c>
+      <c r="BU31" s="3"/>
+      <c r="BV31" s="3"/>
+      <c r="BW31" s="3"/>
+      <c r="BX31" s="4"/>
+      <c r="BY31" s="4"/>
+      <c r="BZ31" s="4"/>
+      <c r="CA31" s="4"/>
     </row>
     <row r="32" spans="1:79">
-      <c r="A32" t="s">
-        <v>27</v>
-      </c>
+      <c r="B32" t="s">
+        <v>18</v>
+      </c>
+      <c r="BU32" s="4"/>
+      <c r="BV32" s="4"/>
+      <c r="BW32" s="4"/>
+      <c r="BX32" s="4"/>
     </row>
     <row r="33" spans="1:103">
       <c r="B33" t="s">
-        <v>28</v>
-      </c>
-      <c r="BU33" s="4"/>
-      <c r="BV33" s="4"/>
-      <c r="BW33" s="4"/>
-      <c r="BX33" s="4"/>
-      <c r="BY33" s="4"/>
-      <c r="BZ33" s="4"/>
-      <c r="CA33" s="4"/>
+        <v>26</v>
+      </c>
+      <c r="BY33" s="6"/>
+      <c r="BZ33" s="6"/>
+      <c r="CA33" s="6"/>
     </row>
     <row r="35" spans="1:103">
       <c r="A35" t="s">

</xml_diff>

<commit_message>
Small changes to the gantt chart
</commit_message>
<xml_diff>
--- a/Documents/Laker Books Gantt Chart.xlsx
+++ b/Documents/Laker Books Gantt Chart.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Phases</t>
   </si>
@@ -115,9 +115,6 @@
   </si>
   <si>
     <t>Work on the email interaction once sold</t>
-  </si>
-  <si>
-    <t>Add ability for seller to set preferred meetup area</t>
   </si>
   <si>
     <t>Deployment and final degbugging and testing</t>
@@ -176,7 +173,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -201,12 +198,6 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF8DB4E2"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -217,7 +208,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="107">
+  <cellStyleXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -325,17 +316,24 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="107">
+  <cellStyles count="115">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -389,6 +387,10 @@
     <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -442,6 +444,10 @@
     <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -771,10 +777,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CZ41"/>
+  <dimension ref="A1:CZ40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BI20" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="BU31" sqref="BU31:BW31"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1242,7 +1248,7 @@
     </row>
     <row r="11" spans="1:104">
       <c r="B11" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
@@ -1372,7 +1378,7 @@
     </row>
     <row r="23" spans="1:79">
       <c r="B23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AT23" s="3"/>
       <c r="AU23" s="3"/>
@@ -1437,13 +1443,13 @@
       <c r="A30" t="s">
         <v>27</v>
       </c>
-      <c r="BU30" s="4"/>
-      <c r="BV30" s="4"/>
-      <c r="BW30" s="4"/>
-      <c r="BX30" s="4"/>
-      <c r="BY30" s="4"/>
-      <c r="BZ30" s="4"/>
-      <c r="CA30" s="4"/>
+      <c r="BU30" s="3"/>
+      <c r="BV30" s="3"/>
+      <c r="BW30" s="3"/>
+      <c r="BX30" s="3"/>
+      <c r="BY30" s="3"/>
+      <c r="BZ30" s="3"/>
+      <c r="CA30" s="3"/>
     </row>
     <row r="31" spans="1:79">
       <c r="B31" t="s">
@@ -1452,63 +1458,80 @@
       <c r="BU31" s="3"/>
       <c r="BV31" s="3"/>
       <c r="BW31" s="3"/>
-      <c r="BX31" s="4"/>
-      <c r="BY31" s="4"/>
-      <c r="BZ31" s="4"/>
-      <c r="CA31" s="4"/>
+      <c r="BX31" s="3"/>
+      <c r="BY31" s="3"/>
+      <c r="BZ31" s="3"/>
+      <c r="CA31" s="3"/>
     </row>
     <row r="32" spans="1:79">
       <c r="B32" t="s">
         <v>18</v>
       </c>
-      <c r="BU32" s="4"/>
-      <c r="BV32" s="4"/>
-      <c r="BW32" s="4"/>
-      <c r="BX32" s="4"/>
-    </row>
-    <row r="33" spans="1:103">
+      <c r="BU32" s="3"/>
+      <c r="BV32" s="3"/>
+      <c r="BW32" s="3"/>
+      <c r="BX32" s="3"/>
+    </row>
+    <row r="33" spans="1:98">
       <c r="B33" t="s">
         <v>26</v>
       </c>
-      <c r="BY33" s="6"/>
-      <c r="BZ33" s="6"/>
-      <c r="CA33" s="6"/>
-    </row>
-    <row r="35" spans="1:103">
+      <c r="BY33" s="5"/>
+      <c r="BZ33" s="5"/>
+      <c r="CA33" s="5"/>
+    </row>
+    <row r="35" spans="1:98">
       <c r="A35" t="s">
         <v>29</v>
       </c>
-      <c r="CB35" s="4"/>
-      <c r="CC35" s="4"/>
-      <c r="CD35" s="4"/>
-      <c r="CE35" s="4"/>
-      <c r="CF35" s="4"/>
-      <c r="CG35" s="4"/>
-      <c r="CH35" s="4"/>
-    </row>
-    <row r="36" spans="1:103">
+      <c r="CB35" s="3"/>
+      <c r="CC35" s="3"/>
+      <c r="CD35" s="3"/>
+      <c r="CE35" s="3"/>
+      <c r="CF35" s="3"/>
+      <c r="CG35" s="3"/>
+      <c r="CH35" s="3"/>
+    </row>
+    <row r="36" spans="1:98">
       <c r="B36" t="s">
         <v>31</v>
       </c>
-      <c r="CB36" s="4"/>
-      <c r="CC36" s="4"/>
-      <c r="CD36" s="4"/>
-    </row>
-    <row r="37" spans="1:103">
-      <c r="B37" t="s">
+      <c r="CB36" s="3"/>
+      <c r="CC36" s="3"/>
+      <c r="CD36" s="3"/>
+      <c r="CE36" s="3"/>
+      <c r="CF36" s="3"/>
+      <c r="CG36" s="3"/>
+      <c r="CH36" s="3"/>
+    </row>
+    <row r="38" spans="1:98">
+      <c r="A38" t="s">
+        <v>30</v>
+      </c>
+      <c r="CI38" s="3"/>
+      <c r="CJ38" s="3"/>
+      <c r="CK38" s="3"/>
+      <c r="CL38" s="3"/>
+      <c r="CM38" s="3"/>
+      <c r="CN38" s="4"/>
+      <c r="CO38" s="4"/>
+      <c r="CP38" s="4"/>
+      <c r="CQ38" s="4"/>
+      <c r="CR38" s="4"/>
+      <c r="CS38" s="4"/>
+      <c r="CT38" s="4"/>
+    </row>
+    <row r="39" spans="1:98">
+      <c r="B39" t="s">
         <v>32</v>
       </c>
-      <c r="CE37" s="4"/>
-      <c r="CF37" s="4"/>
-      <c r="CG37" s="4"/>
-      <c r="CH37" s="4"/>
-    </row>
-    <row r="39" spans="1:103">
-      <c r="A39" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="40" spans="1:103">
+      <c r="CI39" s="3"/>
+      <c r="CJ39" s="3"/>
+      <c r="CK39" s="3"/>
+      <c r="CL39" s="3"/>
+      <c r="CM39" s="3"/>
+    </row>
+    <row r="40" spans="1:98">
       <c r="B40" t="s">
         <v>33</v>
       </c>
@@ -1517,18 +1540,8 @@
       <c r="CP40" s="4"/>
       <c r="CQ40" s="4"/>
       <c r="CR40" s="4"/>
-    </row>
-    <row r="41" spans="1:103">
-      <c r="B41" t="s">
-        <v>34</v>
-      </c>
-      <c r="CS41" s="4"/>
-      <c r="CT41" s="4"/>
-      <c r="CU41" s="4"/>
-      <c r="CV41" s="4"/>
-      <c r="CW41" s="4"/>
-      <c r="CX41" s="4"/>
-      <c r="CY41" s="4"/>
+      <c r="CS40" s="4"/>
+      <c r="CT40" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Changes to documents and addition of final required documents
</commit_message>
<xml_diff>
--- a/Documents/Laker Books Gantt Chart.xlsx
+++ b/Documents/Laker Books Gantt Chart.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14400" tabRatio="500"/>
@@ -120,13 +120,13 @@
     <t>Deployment and final degbugging and testing</t>
   </si>
   <si>
-    <t>If time permits, create iOS and Android application</t>
-  </si>
-  <si>
     <t>Create GUI Skeleton</t>
   </si>
   <si>
     <t>Finish backend functionality</t>
+  </si>
+  <si>
+    <t>Report User Functionality</t>
   </si>
 </sst>
 </file>
@@ -208,8 +208,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="115">
+  <cellStyleXfs count="127">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -333,7 +345,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="115">
+  <cellStyles count="127">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -391,6 +403,12 @@
     <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -448,6 +466,12 @@
     <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -777,10 +801,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CZ40"/>
+  <dimension ref="A1:CZ39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="BS27" sqref="BS27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1248,7 +1272,7 @@
     </row>
     <row r="11" spans="1:104">
       <c r="B11" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
@@ -1378,7 +1402,7 @@
     </row>
     <row r="23" spans="1:79">
       <c r="B23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AT23" s="3"/>
       <c r="AU23" s="3"/>
@@ -1417,6 +1441,8 @@
       <c r="BR26" s="3"/>
       <c r="BS26" s="3"/>
       <c r="BT26" s="3"/>
+      <c r="BU26" s="3"/>
+      <c r="BV26" s="3"/>
     </row>
     <row r="27" spans="1:79">
       <c r="B27" t="s">
@@ -1431,6 +1457,10 @@
       <c r="BP27" s="3"/>
       <c r="BQ27" s="3"/>
       <c r="BR27" s="3"/>
+      <c r="BS27" s="3"/>
+      <c r="BT27" s="3"/>
+      <c r="BU27" s="3"/>
+      <c r="BV27" s="3"/>
     </row>
     <row r="28" spans="1:79">
       <c r="B28" t="s">
@@ -1472,15 +1502,15 @@
       <c r="BW32" s="3"/>
       <c r="BX32" s="3"/>
     </row>
-    <row r="33" spans="1:98">
+    <row r="33" spans="1:104">
       <c r="B33" t="s">
-        <v>26</v>
-      </c>
-      <c r="BY33" s="5"/>
-      <c r="BZ33" s="5"/>
-      <c r="CA33" s="5"/>
-    </row>
-    <row r="35" spans="1:98">
+        <v>35</v>
+      </c>
+      <c r="BY33" s="3"/>
+      <c r="BZ33" s="3"/>
+      <c r="CA33" s="3"/>
+    </row>
+    <row r="35" spans="1:104">
       <c r="A35" t="s">
         <v>29</v>
       </c>
@@ -1491,8 +1521,11 @@
       <c r="CF35" s="3"/>
       <c r="CG35" s="3"/>
       <c r="CH35" s="3"/>
-    </row>
-    <row r="36" spans="1:98">
+      <c r="CI35" s="3"/>
+      <c r="CJ35" s="3"/>
+      <c r="CK35" s="3"/>
+    </row>
+    <row r="36" spans="1:104">
       <c r="B36" t="s">
         <v>31</v>
       </c>
@@ -1504,44 +1537,53 @@
       <c r="CG36" s="3"/>
       <c r="CH36" s="3"/>
     </row>
-    <row r="38" spans="1:98">
+    <row r="37" spans="1:104">
+      <c r="B37" t="s">
+        <v>26</v>
+      </c>
+      <c r="CI37" s="3"/>
+      <c r="CJ37" s="3"/>
+      <c r="CK37" s="3"/>
+    </row>
+    <row r="38" spans="1:104">
       <c r="A38" t="s">
         <v>30</v>
       </c>
-      <c r="CI38" s="3"/>
-      <c r="CJ38" s="3"/>
-      <c r="CK38" s="3"/>
       <c r="CL38" s="3"/>
       <c r="CM38" s="3"/>
-      <c r="CN38" s="4"/>
-      <c r="CO38" s="4"/>
-      <c r="CP38" s="4"/>
+      <c r="CN38" s="3"/>
+      <c r="CO38" s="3"/>
+      <c r="CP38" s="3"/>
       <c r="CQ38" s="4"/>
       <c r="CR38" s="4"/>
       <c r="CS38" s="4"/>
       <c r="CT38" s="4"/>
-    </row>
-    <row r="39" spans="1:98">
+      <c r="CU38" s="4"/>
+      <c r="CV38" s="4"/>
+      <c r="CW38" s="4"/>
+      <c r="CX38" s="4"/>
+      <c r="CY38" s="4"/>
+      <c r="CZ38" s="4"/>
+    </row>
+    <row r="39" spans="1:104">
       <c r="B39" t="s">
         <v>32</v>
       </c>
-      <c r="CI39" s="3"/>
-      <c r="CJ39" s="3"/>
-      <c r="CK39" s="3"/>
       <c r="CL39" s="3"/>
       <c r="CM39" s="3"/>
-    </row>
-    <row r="40" spans="1:98">
-      <c r="B40" t="s">
-        <v>33</v>
-      </c>
-      <c r="CN40" s="4"/>
-      <c r="CO40" s="4"/>
-      <c r="CP40" s="4"/>
-      <c r="CQ40" s="4"/>
-      <c r="CR40" s="4"/>
-      <c r="CS40" s="4"/>
-      <c r="CT40" s="4"/>
+      <c r="CN39" s="3"/>
+      <c r="CO39" s="3"/>
+      <c r="CP39" s="3"/>
+      <c r="CQ39" s="4"/>
+      <c r="CR39" s="4"/>
+      <c r="CS39" s="4"/>
+      <c r="CT39" s="4"/>
+      <c r="CU39" s="4"/>
+      <c r="CV39" s="4"/>
+      <c r="CW39" s="4"/>
+      <c r="CX39" s="4"/>
+      <c r="CY39" s="4"/>
+      <c r="CZ39" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>